<commit_message>
added relative path to signup
</commit_message>
<xml_diff>
--- a/BirdsControl/BirdsControl/login_file.xlsx
+++ b/BirdsControl/BirdsControl/login_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofma\OneDrive\שולחן העבודה\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alter\Desktop\school\Second_Year\Second_semester\testing_and_quallity\BirdsControl\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A81C1D-3F17-4045-A84F-5F6B42189218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BBE61B-3D98-4CB5-AEEE-B64B01433FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="18851" windowHeight="9844" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>lior1234@</t>
+  </si>
+  <si>
+    <t>ritay12</t>
+  </si>
+  <si>
+    <t>ritay12@</t>
   </si>
 </sst>
 </file>
@@ -73,7 +79,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -119,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,16 +421,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.4140625" customWidth="1"/>
-    <col min="3" max="3" width="20.4140625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -537,6 +543,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>311434621</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>